<commit_message>
Changed bunch of shit
New input parameters added, Changed ElementVec to reflect change to
meters, and increment error fixed. More shit added to massX for string
and to coeff matrices to accomodate string
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Younge's</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Length</t>
+  </si>
+  <si>
+    <t>Radius</t>
   </si>
 </sst>
 </file>
@@ -385,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -436,8 +439,8 @@
         <v>1.6553</v>
       </c>
       <c r="F2">
-        <f>E2*937</f>
-        <v>1551.0161000000001</v>
+        <f>E2*937/1000</f>
+        <v>1.5510161</v>
       </c>
       <c r="H2">
         <v>200000000000</v>
@@ -473,6 +476,16 @@
       </c>
       <c r="H6">
         <v>1.4732000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="H8">
+        <v>1.5874999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
on the wideness of the wides make it sider
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="20730" windowHeight="11760"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -69,8 +69,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +190,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -224,6 +225,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -399,19 +401,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -437,7 +439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>6894757290</v>
       </c>
@@ -458,7 +460,7 @@
         <v>200000000000</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -466,7 +468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>470</v>
       </c>
@@ -474,7 +476,7 @@
         <v>1.6442700000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -482,15 +484,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>5.0799999999999998E-2</v>
+        <v>4.4450000000000003E-2</v>
       </c>
       <c r="H6">
         <v>1.4732000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>12</v>
       </c>
@@ -498,7 +500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>1790000</v>
       </c>
@@ -506,32 +508,32 @@
         <v>1.5874999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>16500000</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>5560000</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>24800000</v>
       </c>
@@ -542,24 +544,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
shawty said nigga she with aint shitttt
</commit_message>
<xml_diff>
--- a/InputFile.xlsx
+++ b/InputFile.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Younge's</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Mass</t>
-  </si>
-  <si>
-    <t>Length</t>
   </si>
   <si>
     <t>Radius</t>
@@ -405,12 +402,13 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -489,14 +487,11 @@
         <v>4.4450000000000003E-2</v>
       </c>
       <c r="H6">
-        <v>1.4732000000000001</v>
+        <v>1.5874999999999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -504,13 +499,10 @@
       <c r="B8">
         <v>1790000</v>
       </c>
-      <c r="H8">
-        <v>1.5874999999999999E-3</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,7 +512,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -530,7 +522,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>